<commit_message>
csv read 오류 수정
</commit_message>
<xml_diff>
--- a/document/projectDT.xlsx
+++ b/document/projectDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C\Documents\GitHub\Mandle_10Minute_Game\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A88128D-9491-4762-88C4-9C7FF09C316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510500E6-B117-482C-9496-B193AC08F91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{A908816F-3EB3-47CA-8A2F-AC05E9BE3A54}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{A908816F-3EB3-47CA-8A2F-AC05E9BE3A54}"/>
   </bookViews>
   <sheets>
     <sheet name="EventDT" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="230">
   <si>
     <t>//</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -660,6 +660,241 @@
   </si>
   <si>
     <t>wifi</t>
+  </si>
+  <si>
+    <t>택배기사 채팅 팝업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만에 연락한 친구 채팅 팝업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동창회 회장 채팅 팝업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>택배기사와의 채팅 App 대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>택배기사와 대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>택배기사와 대화종료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>택배기사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만에 연락한 친구 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동창회 회장 친구 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕하세요, 고객님. 배송 도착했는데 문 앞에 두고 갑니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아, 네! 그냥 두고 가주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넵 감사합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넵, 안전하게 놓고 갑니다. 좋은 하루 되세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3124, 3125</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>광고이벤트메세지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만에 연락한 친구 채팅 App대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동창회 회장 채팅 App대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3004, 3123, 3124, 3120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>야 들래야! 오랜만이네 잘 지내냐?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오 오랜만, 나는 잘지내지 너는 어떻게 지내?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그럭저럭 지내고 있어, 너는 어떻게 지내?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실례지만 누구세요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3005, 3127, 3128 , 3129, 3130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만인친구와 대화1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3128, 3129</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만인친구와 대화2</t>
+  </si>
+  <si>
+    <t>오랜만인친구와 대화3</t>
+  </si>
+  <si>
+    <t>오랜만인친구와 대화4</t>
+  </si>
+  <si>
+    <t>오랜만친구 대화종료1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오랜만친구 대화종료2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나도 잘 지내고 있지, 사진 정리하다가 너랑 친구들이랑 같이 여행 갔던거 생각나서 연락했어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그때 재미있었지, 그때 같이 갔던 애들이랑 다같이 만날래?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아하 그렇구나, 오랜만에 다 같이 모여서 만날까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3132, 3133</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아 그러면 다음주 수요일에 만나는 거 어때?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가능할 것 같아 그때 만나자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어 나 그날은 안될 것 같아, 조금 있다가 되는날 알려 줄게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요일은 좀 힘든데 그러면 다음주 금요일은 어때?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3135, 3137</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예전에 너랑 같이 여행 갔던 OO이야 너무 오랜만이라 까먹은거야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장난이야 기억하지 잘 지내?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아 기억났다 순간 누군가 했네 미안하다. 잘 지내?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3139, 3140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋아, 그러면 그날 만나는 걸로 하자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 그러면 되는 날 말해줘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동창회 대화 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동창회 대화 2</t>
+  </si>
+  <si>
+    <t>동창회 대화종료1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동창회 대화종료2</t>
+  </si>
+  <si>
+    <t>들래야! 잘 지내냐? 우리 다음주에 동창회 하는데 올래? 다들 모인다고 해서 연락해봤어!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음..혹시 누구누구 오는지 알 수 있을까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3006, 3143, 3144, 3135, 3136</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 시간 될 것 같아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3144, 3145</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너랑 친했던 XX도 오고, OO도 올거야 다들 너 보고 싶어하더라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 그러면 가는걸로 할게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음…내가 다음주에는 일정이 많아서…안될 것 같아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어.. 다음 주에는 시간이 안될 것 같아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 그러면 오는 걸로 알고 있을게, 조금 있다가 오는 애들 다 정해지면 단톡방 초대해줄게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래 그러면 못 오는 걸로 알고 있을게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -879,7 +1114,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -981,6 +1216,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1331,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774D0F37-8F82-455B-A8BD-E50AA5512BE5}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -1344,7 +1582,8 @@
     <col min="4" max="4" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.69921875" customWidth="1"/>
+    <col min="8" max="8" width="23.19921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.59765625" customWidth="1"/>
     <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
@@ -1421,7 +1660,7 @@
       <c r="B3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -1451,7 +1690,7 @@
       <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
         <v>43</v>
@@ -1477,7 +1716,7 @@
       <c r="B5" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="12" t="s">
         <v>164</v>
       </c>
@@ -1499,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="14"/>
-      <c r="C6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="15" t="s">
         <v>165</v>
       </c>
@@ -1680,89 +1919,76 @@
       <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="B14" s="5">
+        <v>1006</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="16">
+        <v>2002</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="5">
-        <v>1101</v>
+        <v>1007</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>171</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="16">
-        <v>2001</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+        <v>2002</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" s="5">
-        <v>1102</v>
+        <v>1008</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F16" s="16">
         <v>2002</v>
       </c>
-      <c r="G16" s="16">
-        <v>4002</v>
-      </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="B17" s="5">
-        <v>1103</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="16">
-        <v>2002</v>
-      </c>
-      <c r="G17" s="16">
-        <v>4001</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:11">
       <c r="B18" s="5">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1771,108 +1997,241 @@
         <v>17</v>
       </c>
       <c r="F18" s="16">
-        <v>2004</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>109</v>
-      </c>
+        <v>2001</v>
+      </c>
+      <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
-      <c r="J18" s="16">
-        <v>4001</v>
-      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="B19" s="5">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="16">
-        <v>2003</v>
-      </c>
-      <c r="G19" s="16"/>
+        <v>2002</v>
+      </c>
+      <c r="G19" s="16">
+        <v>4002</v>
+      </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:11" ht="33" customHeight="1">
       <c r="B20" s="5">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F20" s="16">
-        <v>2005</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>2002</v>
+      </c>
+      <c r="G20" s="16">
+        <v>4001</v>
+      </c>
       <c r="H20" s="16"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:11">
       <c r="B21" s="5">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F21" s="16">
         <v>2004</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="B22" s="5">
+        <v>1105</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="16">
+        <v>2003</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" ht="69.599999999999994">
+      <c r="B23" s="5">
+        <v>1106</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="16">
+        <v>2005</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="B24" s="5">
+        <v>1107</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="16">
+        <v>2004</v>
+      </c>
+      <c r="G24" s="5">
         <v>3003</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" s="5">
+        <v>1108</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="16">
+        <v>2004</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="J25">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="B26" s="5">
+        <v>1109</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="16">
+        <v>2004</v>
+      </c>
+      <c r="G26" t="s">
+        <v>192</v>
+      </c>
+      <c r="J26">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="B27" s="5">
+        <v>1110</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2004</v>
+      </c>
+      <c r="G27" t="s">
+        <v>221</v>
+      </c>
+      <c r="J27">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="B23" s="5">
+    <row r="31" spans="1:11">
+      <c r="B31" s="5">
         <v>4004</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C31" t="s">
         <v>159</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F31" s="16">
         <v>2005</v>
       </c>
     </row>
@@ -1887,16 +2246,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2797C8FA-D3B7-48B0-ACA1-D58AE830954C}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1928,7 +2287,7 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1939,7 +2298,7 @@
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
@@ -1948,7 +2307,7 @@
       <c r="B5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
@@ -1957,7 +2316,7 @@
       <c r="B6" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -2003,210 +2362,466 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34.799999999999997">
+      <c r="B12">
+        <v>3004</v>
+      </c>
+      <c r="C12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="B13">
-        <v>3101</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>114</v>
+        <v>3005</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14">
-        <v>3102</v>
+        <v>3006</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="B15">
-        <v>3103</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="34.799999999999997">
       <c r="B16">
-        <v>3104</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
+        <v>3101</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17">
-        <v>3105</v>
+        <v>3102</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18">
-        <v>3106</v>
+        <v>3103</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19">
-        <v>3107</v>
+        <v>3104</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20">
-        <v>3108</v>
+        <v>3105</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21">
-        <v>3109</v>
+        <v>3106</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22">
-        <v>3110</v>
+        <v>3107</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23">
-        <v>3111</v>
+        <v>3108</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24">
-        <v>3112</v>
+        <v>3109</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25">
-        <v>3113</v>
+        <v>3110</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26">
-        <v>3114</v>
+        <v>3111</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27">
-        <v>3115</v>
+        <v>3112</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28">
-        <v>3116</v>
+        <v>3113</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="B29">
-        <v>3117</v>
+        <v>3114</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="2:3">
       <c r="B30">
-        <v>3118</v>
+        <v>3115</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="2:3">
       <c r="B31">
-        <v>3119</v>
+        <v>3116</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32">
+        <v>3117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33">
+        <v>3118</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34">
+        <v>3119</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35">
         <v>3120</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="B33">
+    <row r="36" spans="2:3">
+      <c r="B36">
         <v>3121</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C36" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="B34">
+    <row r="37" spans="2:3">
+      <c r="B37">
         <v>3122</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="38" spans="2:3">
+      <c r="B38">
+        <v>3123</v>
+      </c>
+      <c r="C38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39">
+        <v>3124</v>
+      </c>
+      <c r="C39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40">
+        <v>3125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41">
+        <v>3126</v>
+      </c>
+      <c r="C41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42">
+        <v>3127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43">
+        <v>3128</v>
+      </c>
+      <c r="C43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44">
+        <v>3129</v>
+      </c>
+      <c r="C44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45">
+        <v>3130</v>
+      </c>
+      <c r="C45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46">
+        <v>3131</v>
+      </c>
+      <c r="C46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47">
+        <v>3132</v>
+      </c>
+      <c r="C47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48">
+        <v>3133</v>
+      </c>
+      <c r="C48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49">
+        <v>3134</v>
+      </c>
+      <c r="C49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50">
+        <v>3135</v>
+      </c>
+      <c r="C50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51">
+        <v>3136</v>
+      </c>
+      <c r="C51" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52">
+        <v>3137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53">
+        <v>3138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54">
+        <v>3139</v>
+      </c>
+      <c r="C54" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3">
+      <c r="B55">
+        <v>3140</v>
+      </c>
+      <c r="C55" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56">
+        <v>3141</v>
+      </c>
+      <c r="C56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57">
+        <v>3142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58">
+        <v>3143</v>
+      </c>
+      <c r="C58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59">
+        <v>3144</v>
+      </c>
+      <c r="C59" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60">
+        <v>3145</v>
+      </c>
+      <c r="C60" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61">
+        <v>3146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62">
+        <v>3147</v>
+      </c>
+      <c r="C62" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3">
+      <c r="B63">
+        <v>3148</v>
+      </c>
+      <c r="C63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3">
+      <c r="B64">
+        <v>3149</v>
+      </c>
+      <c r="C64" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="B65">
+        <v>3150</v>
+      </c>
+      <c r="C65" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="B66">
+        <v>3151</v>
+      </c>
+      <c r="C66" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="B36">
+    <row r="69" spans="1:3">
+      <c r="B69">
         <v>4001</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C69" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="B37">
+    <row r="70" spans="1:3">
+      <c r="B70">
         <v>4002</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C70" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2223,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7ED222-C632-437F-9F99-BE16CE033DC8}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2261,7 +2876,7 @@
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2272,7 +2887,7 @@
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
@@ -2281,14 +2896,14 @@
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="38"/>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
@@ -2376,16 +2991,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AABC80-77F5-4366-AF3C-51BE0B577C17}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="8.69921875" style="5"/>
-    <col min="2" max="3" width="14.19921875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" style="5" customWidth="1"/>
     <col min="4" max="4" width="16.69921875" style="5" customWidth="1"/>
     <col min="5" max="5" width="17" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.69921875" style="5" customWidth="1"/>
@@ -2723,18 +3339,260 @@
       <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="5">
+        <v>4008</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="5">
+        <v>4009</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3123</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="5">
+        <v>4010</v>
+      </c>
+      <c r="I15" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="5">
+        <v>4010</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="B17" s="5">
+        <v>4011</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3127</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4012</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3130</v>
+      </c>
+      <c r="H17" s="5">
+        <v>4014</v>
+      </c>
+      <c r="I17" s="5">
+        <v>50</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="5">
+        <v>4012</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3131</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="5">
+        <v>4013</v>
+      </c>
+      <c r="I18" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="B19" s="5">
+        <v>4013</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3134</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="5">
+        <v>4015</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3136</v>
+      </c>
+      <c r="H19" s="5">
+        <v>4016</v>
+      </c>
+      <c r="I19" s="5">
+        <v>20</v>
+      </c>
+      <c r="J19" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="B20" s="5">
+        <v>4014</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="5">
+        <v>3138</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="5">
+        <v>4012</v>
+      </c>
+      <c r="I20" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="B21" s="5">
+        <v>4015</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="B22" s="5">
+        <v>4016</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="B23" s="5">
+        <v>4017</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3143</v>
+      </c>
+      <c r="E23" s="5">
+        <v>3146</v>
+      </c>
+      <c r="F23" s="5">
+        <v>4019</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4018</v>
+      </c>
+      <c r="I23" s="5">
+        <v>100</v>
+      </c>
+      <c r="J23" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="B24" s="5">
+        <v>4018</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3147</v>
+      </c>
+      <c r="E24" s="5">
+        <v>3148</v>
+      </c>
+      <c r="F24" s="5">
+        <v>4019</v>
+      </c>
+      <c r="G24" s="5">
+        <v>3149</v>
+      </c>
+      <c r="H24" s="5">
+        <v>4020</v>
+      </c>
+      <c r="I24" s="5">
+        <v>50</v>
+      </c>
+      <c r="J24" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25" s="5">
+        <v>4019</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D25" s="5">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" s="5">
+        <v>4020</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="34.799999999999997">
-      <c r="B15" s="5">
+    <row r="30" spans="1:10">
+      <c r="B30" s="5">
         <v>10001</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D30" s="5">
         <v>3101</v>
       </c>
     </row>

</xml_diff>